<commit_message>
test: simplify the timeout logic.
Change-Id: I0c253629b983f2813237536e6e2c6d04d5b97dd1
</commit_message>
<xml_diff>
--- a/test/data/convert-to.xlsx
+++ b/test/data/convert-to.xlsx
@@ -391,9 +391,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>427680</xdr:colOff>
+      <xdr:colOff>427320</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>74880</xdr:rowOff>
+      <xdr:rowOff>74520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -402,8 +402,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2692080" y="876240"/>
-          <a:ext cx="1799280" cy="1799280"/>
+          <a:off x="2600640" y="876240"/>
+          <a:ext cx="1738080" cy="1798920"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -437,10 +437,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.69921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>